<commit_message>
More work on sudoku
</commit_message>
<xml_diff>
--- a/linqpad/problems.xlsx
+++ b/linqpad/problems.xlsx
@@ -1,38 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dev\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\git\github\bcbowen\leetcode\linqpad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BE7582-546D-44DA-A75E-698260FBC055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBF303F-EBBD-4888-99E8-7E87678312A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="1980" windowWidth="22095" windowHeight="12135" activeTab="3" xr2:uid="{F214241B-62AE-4F36-B27B-56072FB5EA56}"/>
+    <workbookView xWindow="1365" yWindow="1230" windowWidth="28800" windowHeight="11295" activeTab="4" xr2:uid="{F214241B-62AE-4F36-B27B-56072FB5EA56}"/>
   </bookViews>
   <sheets>
     <sheet name="221" sheetId="1" r:id="rId1"/>
     <sheet name="322" sheetId="2" r:id="rId2"/>
     <sheet name="835" sheetId="3" r:id="rId3"/>
     <sheet name="48" sheetId="4" r:id="rId4"/>
+    <sheet name="37" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -93,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +93,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -151,16 +148,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1794,7 +1969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CFA318-E6AB-4515-A0C9-0C5BA50F5836}">
   <dimension ref="C7:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1919,4 +2094,338 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8140810B-53E0-4C95-B8FE-5282839B524E}">
+  <dimension ref="B3:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>4</v>
+      </c>
+      <c r="F4" s="8">
+        <v>6</v>
+      </c>
+      <c r="G4" s="6">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7">
+        <v>8</v>
+      </c>
+      <c r="I4" s="8">
+        <v>9</v>
+      </c>
+      <c r="J4" s="9">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>6</v>
+      </c>
+      <c r="D5" s="11">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13">
+        <v>5</v>
+      </c>
+      <c r="I5" s="14">
+        <v>3</v>
+      </c>
+      <c r="J5" s="11">
+        <v>4</v>
+      </c>
+      <c r="K5" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>9</v>
+      </c>
+      <c r="E6" s="17">
+        <v>8</v>
+      </c>
+      <c r="F6" s="15">
+        <v>3</v>
+      </c>
+      <c r="G6" s="18">
+        <v>4</v>
+      </c>
+      <c r="H6" s="19">
+        <v>2</v>
+      </c>
+      <c r="I6" s="15">
+        <v>5</v>
+      </c>
+      <c r="J6" s="16">
+        <v>6</v>
+      </c>
+      <c r="K6" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9</v>
+      </c>
+      <c r="F7" s="8">
+        <v>7</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4</v>
+      </c>
+      <c r="J7" s="9">
+        <v>2</v>
+      </c>
+      <c r="K7" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="12">
+        <v>6</v>
+      </c>
+      <c r="F8" s="10">
+        <v>8</v>
+      </c>
+      <c r="G8" s="11">
+        <v>5</v>
+      </c>
+      <c r="H8" s="13">
+        <v>3</v>
+      </c>
+      <c r="I8" s="14">
+        <v>7</v>
+      </c>
+      <c r="J8" s="11">
+        <v>9</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="21">
+        <v>7</v>
+      </c>
+      <c r="D9" s="22">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23">
+        <v>3</v>
+      </c>
+      <c r="F9" s="15">
+        <v>9</v>
+      </c>
+      <c r="G9" s="16">
+        <v>2</v>
+      </c>
+      <c r="H9" s="19">
+        <v>4</v>
+      </c>
+      <c r="I9" s="15">
+        <v>8</v>
+      </c>
+      <c r="J9" s="18">
+        <v>5</v>
+      </c>
+      <c r="K9" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>3</v>
+      </c>
+      <c r="H10" s="7">
+        <v>7</v>
+      </c>
+      <c r="I10" s="5">
+        <v>2</v>
+      </c>
+      <c r="J10" s="6">
+        <v>8</v>
+      </c>
+      <c r="K10" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2</v>
+      </c>
+      <c r="D11" s="11">
+        <v>8</v>
+      </c>
+      <c r="E11" s="12">
+        <v>7</v>
+      </c>
+      <c r="F11" s="10">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>9</v>
+      </c>
+      <c r="I11" s="14">
+        <v>6</v>
+      </c>
+      <c r="J11" s="11">
+        <v>3</v>
+      </c>
+      <c r="K11" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="15">
+        <v>3</v>
+      </c>
+      <c r="D12" s="18">
+        <v>4</v>
+      </c>
+      <c r="E12" s="19">
+        <v>5</v>
+      </c>
+      <c r="F12" s="15">
+        <v>2</v>
+      </c>
+      <c r="G12" s="16">
+        <v>8</v>
+      </c>
+      <c r="H12" s="19">
+        <v>6</v>
+      </c>
+      <c r="I12" s="15">
+        <v>1</v>
+      </c>
+      <c r="J12" s="16">
+        <v>7</v>
+      </c>
+      <c r="K12" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sudoku... solving some test cases, need more work
</commit_message>
<xml_diff>
--- a/linqpad/problems.xlsx
+++ b/linqpad/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\git\github\bcbowen\leetcode\linqpad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBF303F-EBBD-4888-99E8-7E87678312A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D08033-617B-4014-86AC-456440E43EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="1230" windowWidth="28800" windowHeight="11295" activeTab="4" xr2:uid="{F214241B-62AE-4F36-B27B-56072FB5EA56}"/>
+    <workbookView xWindow="-915" yWindow="-75" windowWidth="28800" windowHeight="11295" activeTab="4" xr2:uid="{F214241B-62AE-4F36-B27B-56072FB5EA56}"/>
   </bookViews>
   <sheets>
     <sheet name="221" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>matrix</t>
   </si>
@@ -78,12 +78,24 @@
   <si>
     <t>12</t>
   </si>
+  <si>
+    <t>Init</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Cols</t>
+  </si>
+  <si>
+    <t>Sections</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +112,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -307,11 +325,172 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -336,6 +515,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2098,15 +2310,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8140810B-53E0-4C95-B8FE-5282839B524E}">
-  <dimension ref="B3:K13"/>
+  <dimension ref="B3:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="AG10" workbookViewId="0">
+      <selection activeCell="BB28" sqref="BB28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="23" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>0</v>
       </c>
@@ -2135,7 +2350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -2167,7 +2382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -2199,7 +2414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -2231,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -2263,7 +2478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>4</v>
       </c>
@@ -2295,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
@@ -2327,7 +2542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>6</v>
       </c>
@@ -2359,7 +2574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>7</v>
       </c>
@@ -2391,7 +2606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>8</v>
       </c>
@@ -2423,7 +2638,1365 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:47" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
+      </c>
+      <c r="K17">
+        <v>8</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>3</v>
+      </c>
+      <c r="S17">
+        <v>4</v>
+      </c>
+      <c r="T17">
+        <v>5</v>
+      </c>
+      <c r="U17">
+        <v>6</v>
+      </c>
+      <c r="V17">
+        <v>7</v>
+      </c>
+      <c r="W17">
+        <v>8</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <v>3</v>
+      </c>
+      <c r="AD17">
+        <v>4</v>
+      </c>
+      <c r="AE17">
+        <v>5</v>
+      </c>
+      <c r="AF17">
+        <v>6</v>
+      </c>
+      <c r="AG17">
+        <v>7</v>
+      </c>
+      <c r="AH17">
+        <v>8</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>1</v>
+      </c>
+      <c r="AM17">
+        <v>2</v>
+      </c>
+      <c r="AN17">
+        <v>3</v>
+      </c>
+      <c r="AO17">
+        <v>4</v>
+      </c>
+      <c r="AP17">
+        <v>5</v>
+      </c>
+      <c r="AQ17">
+        <v>6</v>
+      </c>
+      <c r="AR17">
+        <v>7</v>
+      </c>
+      <c r="AS17">
+        <v>8</v>
+      </c>
+      <c r="AU17">
+        <v>0</v>
+      </c>
+      <c r="AV17">
+        <v>1</v>
+      </c>
+      <c r="AW17">
+        <v>2</v>
+      </c>
+      <c r="AX17">
+        <v>3</v>
+      </c>
+      <c r="AY17">
+        <v>4</v>
+      </c>
+      <c r="AZ17">
+        <v>5</v>
+      </c>
+      <c r="BA17">
+        <v>6</v>
+      </c>
+      <c r="BB17">
+        <v>7</v>
+      </c>
+      <c r="BC17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26">
+        <v>9</v>
+      </c>
+      <c r="F18" s="24">
+        <v>7</v>
+      </c>
+      <c r="G18" s="25">
+        <v>4</v>
+      </c>
+      <c r="H18" s="26">
+        <v>8</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26"/>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="24">
+        <v>123456789</v>
+      </c>
+      <c r="P18" s="25">
+        <v>123456789</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>9</v>
+      </c>
+      <c r="R18" s="36">
+        <v>7</v>
+      </c>
+      <c r="S18" s="25">
+        <v>4</v>
+      </c>
+      <c r="T18" s="39">
+        <v>8</v>
+      </c>
+      <c r="U18" s="24">
+        <v>123456789</v>
+      </c>
+      <c r="V18" s="25">
+        <v>123456789</v>
+      </c>
+      <c r="W18" s="26">
+        <v>123456789</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="24">
+        <v>12356</v>
+      </c>
+      <c r="AA18" s="25">
+        <v>12356</v>
+      </c>
+      <c r="AB18" s="26">
+        <v>9</v>
+      </c>
+      <c r="AC18" s="36">
+        <v>7</v>
+      </c>
+      <c r="AD18" s="25">
+        <v>4</v>
+      </c>
+      <c r="AE18" s="39">
+        <v>8</v>
+      </c>
+      <c r="AF18" s="24">
+        <v>12356</v>
+      </c>
+      <c r="AG18" s="25">
+        <v>12356</v>
+      </c>
+      <c r="AH18" s="26">
+        <v>12356</v>
+      </c>
+      <c r="AK18" s="24">
+        <v>12356</v>
+      </c>
+      <c r="AL18" s="25">
+        <v>135</v>
+      </c>
+      <c r="AM18" s="26">
+        <v>9</v>
+      </c>
+      <c r="AN18" s="36">
+        <v>7</v>
+      </c>
+      <c r="AO18" s="25">
+        <v>4</v>
+      </c>
+      <c r="AP18" s="39">
+        <v>8</v>
+      </c>
+      <c r="AQ18" s="24">
+        <v>16</v>
+      </c>
+      <c r="AR18" s="25">
+        <v>1356</v>
+      </c>
+      <c r="AS18" s="26">
+        <v>1235</v>
+      </c>
+      <c r="AU18" s="24">
+        <v>356</v>
+      </c>
+      <c r="AV18" s="25">
+        <v>135</v>
+      </c>
+      <c r="AW18" s="26">
+        <v>9</v>
+      </c>
+      <c r="AX18" s="36">
+        <v>7</v>
+      </c>
+      <c r="AY18" s="25">
+        <v>4</v>
+      </c>
+      <c r="AZ18" s="39">
+        <v>8</v>
+      </c>
+      <c r="BA18" s="24">
+        <v>16</v>
+      </c>
+      <c r="BB18" s="25">
+        <v>135</v>
+      </c>
+      <c r="BC18" s="26">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="27">
+        <v>7</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19" s="27">
+        <v>7</v>
+      </c>
+      <c r="P19" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="Q19" s="29">
+        <v>123456789</v>
+      </c>
+      <c r="R19" s="37">
+        <v>123456789</v>
+      </c>
+      <c r="S19" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="T19" s="40">
+        <v>123456789</v>
+      </c>
+      <c r="U19" s="27">
+        <v>123456789</v>
+      </c>
+      <c r="V19" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="W19" s="29">
+        <v>123456789</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="27">
+        <v>7</v>
+      </c>
+      <c r="AA19" s="28">
+        <v>12345689</v>
+      </c>
+      <c r="AB19" s="29">
+        <v>12345689</v>
+      </c>
+      <c r="AC19" s="37">
+        <v>12345689</v>
+      </c>
+      <c r="AD19" s="28">
+        <v>12345689</v>
+      </c>
+      <c r="AE19" s="40">
+        <v>12345689</v>
+      </c>
+      <c r="AF19" s="27">
+        <v>12345689</v>
+      </c>
+      <c r="AG19" s="28">
+        <v>12345689</v>
+      </c>
+      <c r="AH19" s="29">
+        <v>12345689</v>
+      </c>
+      <c r="AK19" s="27">
+        <v>7</v>
+      </c>
+      <c r="AL19" s="28">
+        <v>13458</v>
+      </c>
+      <c r="AM19" s="29">
+        <v>12356</v>
+      </c>
+      <c r="AN19" s="37">
+        <v>4569</v>
+      </c>
+      <c r="AO19" s="28">
+        <v>235689</v>
+      </c>
+      <c r="AP19" s="40">
+        <v>1246</v>
+      </c>
+      <c r="AQ19" s="27">
+        <v>1468</v>
+      </c>
+      <c r="AR19" s="28">
+        <v>13568</v>
+      </c>
+      <c r="AS19" s="29">
+        <v>1234589</v>
+      </c>
+      <c r="AU19" s="27">
+        <v>7</v>
+      </c>
+      <c r="AV19" s="28">
+        <v>13458</v>
+      </c>
+      <c r="AW19" s="29">
+        <v>135</v>
+      </c>
+      <c r="AX19" s="49">
+        <v>6</v>
+      </c>
+      <c r="AY19" s="28">
+        <v>35</v>
+      </c>
+      <c r="AZ19" s="53">
+        <v>2</v>
+      </c>
+      <c r="BA19" s="27">
+        <v>148</v>
+      </c>
+      <c r="BB19" s="28">
+        <v>1358</v>
+      </c>
+      <c r="BC19" s="29">
+        <v>3459</v>
+      </c>
+    </row>
+    <row r="20" spans="2:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31">
+        <v>2</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="30">
+        <v>1</v>
+      </c>
+      <c r="G20" s="31"/>
+      <c r="H20" s="32">
+        <v>9</v>
+      </c>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="32"/>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20" s="30">
+        <v>123456789</v>
+      </c>
+      <c r="P20" s="31">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="32">
+        <v>123456789</v>
+      </c>
+      <c r="R20" s="38">
+        <v>1</v>
+      </c>
+      <c r="S20" s="31">
+        <v>123456789</v>
+      </c>
+      <c r="T20" s="41">
+        <v>9</v>
+      </c>
+      <c r="U20" s="30">
+        <v>123456789</v>
+      </c>
+      <c r="V20" s="31">
+        <v>123456789</v>
+      </c>
+      <c r="W20" s="32">
+        <v>123456789</v>
+      </c>
+      <c r="Y20">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="30">
+        <v>345678</v>
+      </c>
+      <c r="AA20" s="31">
+        <v>2</v>
+      </c>
+      <c r="AB20" s="32">
+        <v>345678</v>
+      </c>
+      <c r="AC20" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="31">
+        <v>345678</v>
+      </c>
+      <c r="AE20" s="41">
+        <v>9</v>
+      </c>
+      <c r="AF20" s="30">
+        <v>345678</v>
+      </c>
+      <c r="AG20" s="31">
+        <v>345678</v>
+      </c>
+      <c r="AH20" s="32">
+        <v>345678</v>
+      </c>
+      <c r="AK20" s="30">
+        <v>34568</v>
+      </c>
+      <c r="AL20" s="31">
+        <v>2</v>
+      </c>
+      <c r="AM20" s="32">
+        <v>356</v>
+      </c>
+      <c r="AN20" s="38">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="31">
+        <v>3568</v>
+      </c>
+      <c r="AP20" s="41">
+        <v>9</v>
+      </c>
+      <c r="AQ20" s="30">
+        <v>4678</v>
+      </c>
+      <c r="AR20" s="31">
+        <v>35678</v>
+      </c>
+      <c r="AS20" s="32">
+        <v>34578</v>
+      </c>
+      <c r="AU20" s="30">
+        <v>34568</v>
+      </c>
+      <c r="AV20" s="31">
+        <v>2</v>
+      </c>
+      <c r="AW20" s="32">
+        <v>356</v>
+      </c>
+      <c r="AX20" s="38">
+        <v>1</v>
+      </c>
+      <c r="AY20" s="31">
+        <v>35</v>
+      </c>
+      <c r="AZ20" s="41">
+        <v>9</v>
+      </c>
+      <c r="BA20" s="30">
+        <v>4678</v>
+      </c>
+      <c r="BB20" s="31">
+        <v>3578</v>
+      </c>
+      <c r="BC20" s="32">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="2:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26">
+        <v>7</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="24">
+        <v>2</v>
+      </c>
+      <c r="J21" s="25">
+        <v>4</v>
+      </c>
+      <c r="K21" s="26"/>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21" s="42">
+        <v>123456789</v>
+      </c>
+      <c r="P21" s="43">
+        <v>123456789</v>
+      </c>
+      <c r="Q21" s="44">
+        <v>7</v>
+      </c>
+      <c r="R21" s="45">
+        <v>123456789</v>
+      </c>
+      <c r="S21" s="43">
+        <v>123456789</v>
+      </c>
+      <c r="T21" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="U21" s="42">
+        <v>2</v>
+      </c>
+      <c r="V21" s="43">
+        <v>4</v>
+      </c>
+      <c r="W21" s="44">
+        <v>123456789</v>
+      </c>
+      <c r="Y21">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="42">
+        <v>135689</v>
+      </c>
+      <c r="AA21" s="43">
+        <v>135689</v>
+      </c>
+      <c r="AB21" s="44">
+        <v>7</v>
+      </c>
+      <c r="AC21" s="45">
+        <v>135689</v>
+      </c>
+      <c r="AD21" s="43">
+        <v>135689</v>
+      </c>
+      <c r="AE21" s="46">
+        <v>135689</v>
+      </c>
+      <c r="AF21" s="42">
+        <v>2</v>
+      </c>
+      <c r="AG21" s="43">
+        <v>4</v>
+      </c>
+      <c r="AH21" s="44">
+        <v>135689</v>
+      </c>
+      <c r="AK21" s="42">
+        <v>135689</v>
+      </c>
+      <c r="AL21" s="43">
+        <v>1358</v>
+      </c>
+      <c r="AM21" s="44">
+        <v>7</v>
+      </c>
+      <c r="AN21" s="45">
+        <v>569</v>
+      </c>
+      <c r="AO21" s="43">
+        <v>5689</v>
+      </c>
+      <c r="AP21" s="46">
+        <v>16</v>
+      </c>
+      <c r="AQ21" s="42">
+        <v>2</v>
+      </c>
+      <c r="AR21" s="43">
+        <v>4</v>
+      </c>
+      <c r="AS21" s="44">
+        <v>13589</v>
+      </c>
+      <c r="AU21" s="42">
+        <v>35</v>
+      </c>
+      <c r="AV21" s="43">
+        <v>35</v>
+      </c>
+      <c r="AW21" s="44">
+        <v>7</v>
+      </c>
+      <c r="AX21" s="52">
+        <v>9</v>
+      </c>
+      <c r="AY21" s="43">
+        <v>58</v>
+      </c>
+      <c r="AZ21" s="50">
+        <v>6</v>
+      </c>
+      <c r="BA21" s="42">
+        <v>2</v>
+      </c>
+      <c r="BB21" s="43">
+        <v>4</v>
+      </c>
+      <c r="BC21" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28">
+        <v>6</v>
+      </c>
+      <c r="E22" s="29">
+        <v>4</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28">
+        <v>1</v>
+      </c>
+      <c r="H22" s="29"/>
+      <c r="I22" s="27">
+        <v>5</v>
+      </c>
+      <c r="J22" s="28">
+        <v>9</v>
+      </c>
+      <c r="K22" s="29"/>
+      <c r="N22">
+        <v>4</v>
+      </c>
+      <c r="O22" s="27">
+        <v>123456789</v>
+      </c>
+      <c r="P22" s="28">
+        <v>6</v>
+      </c>
+      <c r="Q22" s="29">
+        <v>4</v>
+      </c>
+      <c r="R22" s="37">
+        <v>123456789</v>
+      </c>
+      <c r="S22" s="28">
+        <v>1</v>
+      </c>
+      <c r="T22" s="40">
+        <v>123456789</v>
+      </c>
+      <c r="U22" s="27">
+        <v>5</v>
+      </c>
+      <c r="V22" s="28">
+        <v>9</v>
+      </c>
+      <c r="W22" s="29">
+        <v>123456789</v>
+      </c>
+      <c r="Y22">
+        <v>4</v>
+      </c>
+      <c r="Z22" s="27">
+        <v>2378</v>
+      </c>
+      <c r="AA22" s="28">
+        <v>6</v>
+      </c>
+      <c r="AB22" s="29">
+        <v>4</v>
+      </c>
+      <c r="AC22" s="37">
+        <v>2378</v>
+      </c>
+      <c r="AD22" s="28">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="40">
+        <v>2378</v>
+      </c>
+      <c r="AF22" s="27">
+        <v>5</v>
+      </c>
+      <c r="AG22" s="28">
+        <v>9</v>
+      </c>
+      <c r="AH22" s="29">
+        <v>2378</v>
+      </c>
+      <c r="AK22" s="27">
+        <v>28</v>
+      </c>
+      <c r="AL22" s="28">
+        <v>6</v>
+      </c>
+      <c r="AM22" s="29">
+        <v>4</v>
+      </c>
+      <c r="AN22" s="49">
+        <v>3</v>
+      </c>
+      <c r="AO22" s="28">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="40">
+        <v>27</v>
+      </c>
+      <c r="AQ22" s="27">
+        <v>5</v>
+      </c>
+      <c r="AR22" s="28">
+        <v>9</v>
+      </c>
+      <c r="AS22" s="29">
+        <v>278</v>
+      </c>
+      <c r="AU22" s="14">
+        <v>2</v>
+      </c>
+      <c r="AV22" s="28">
+        <v>6</v>
+      </c>
+      <c r="AW22" s="29">
+        <v>4</v>
+      </c>
+      <c r="AX22" s="49">
+        <v>3</v>
+      </c>
+      <c r="AY22" s="28">
+        <v>1</v>
+      </c>
+      <c r="AZ22" s="53">
+        <v>7</v>
+      </c>
+      <c r="BA22" s="27">
+        <v>5</v>
+      </c>
+      <c r="BB22" s="28">
+        <v>9</v>
+      </c>
+      <c r="BC22" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34">
+        <v>9</v>
+      </c>
+      <c r="E23" s="35">
+        <v>8</v>
+      </c>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="30">
+        <v>3</v>
+      </c>
+      <c r="J23" s="31"/>
+      <c r="K23" s="32"/>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="O23" s="33">
+        <v>123456789</v>
+      </c>
+      <c r="P23" s="34">
+        <v>9</v>
+      </c>
+      <c r="Q23" s="35">
+        <v>8</v>
+      </c>
+      <c r="R23" s="47">
+        <v>123456789</v>
+      </c>
+      <c r="S23" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="T23" s="48">
+        <v>123456789</v>
+      </c>
+      <c r="U23" s="33">
+        <v>3</v>
+      </c>
+      <c r="V23" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="W23" s="35">
+        <v>123456789</v>
+      </c>
+      <c r="Y23">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="33">
+        <v>124567</v>
+      </c>
+      <c r="AA23" s="34">
+        <v>9</v>
+      </c>
+      <c r="AB23" s="35">
+        <v>8</v>
+      </c>
+      <c r="AC23" s="47">
+        <v>124567</v>
+      </c>
+      <c r="AD23" s="34">
+        <v>124567</v>
+      </c>
+      <c r="AE23" s="48">
+        <v>124567</v>
+      </c>
+      <c r="AF23" s="33">
+        <v>3</v>
+      </c>
+      <c r="AG23" s="34">
+        <v>124567</v>
+      </c>
+      <c r="AH23" s="35">
+        <v>124567</v>
+      </c>
+      <c r="AK23" s="33">
+        <v>12456</v>
+      </c>
+      <c r="AL23" s="34">
+        <v>9</v>
+      </c>
+      <c r="AM23" s="35">
+        <v>8</v>
+      </c>
+      <c r="AN23" s="47">
+        <v>456</v>
+      </c>
+      <c r="AO23" s="34">
+        <v>256</v>
+      </c>
+      <c r="AP23" s="48">
+        <v>12467</v>
+      </c>
+      <c r="AQ23" s="33">
+        <v>3</v>
+      </c>
+      <c r="AR23" s="34">
+        <v>1567</v>
+      </c>
+      <c r="AS23" s="35">
+        <v>12457</v>
+      </c>
+      <c r="AU23" s="55">
+        <v>1</v>
+      </c>
+      <c r="AV23" s="34">
+        <v>9</v>
+      </c>
+      <c r="AW23" s="35">
+        <v>8</v>
+      </c>
+      <c r="AX23" s="51">
+        <v>5</v>
+      </c>
+      <c r="AY23" s="22">
+        <v>2</v>
+      </c>
+      <c r="AZ23" s="54">
+        <v>4</v>
+      </c>
+      <c r="BA23" s="33">
+        <v>3</v>
+      </c>
+      <c r="BB23" s="22">
+        <v>6</v>
+      </c>
+      <c r="BC23" s="23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="24">
+        <v>8</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26">
+        <v>3</v>
+      </c>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25">
+        <v>2</v>
+      </c>
+      <c r="K24" s="26"/>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24" s="24">
+        <v>123456789</v>
+      </c>
+      <c r="P24" s="25">
+        <v>123456789</v>
+      </c>
+      <c r="Q24" s="26">
+        <v>123456789</v>
+      </c>
+      <c r="R24" s="36">
+        <v>8</v>
+      </c>
+      <c r="S24" s="25">
+        <v>123456789</v>
+      </c>
+      <c r="T24" s="39">
+        <v>3</v>
+      </c>
+      <c r="U24" s="24">
+        <v>123456789</v>
+      </c>
+      <c r="V24" s="25">
+        <v>2</v>
+      </c>
+      <c r="W24" s="26">
+        <v>123456789</v>
+      </c>
+      <c r="Y24">
+        <v>6</v>
+      </c>
+      <c r="Z24" s="24">
+        <v>145679</v>
+      </c>
+      <c r="AA24" s="25">
+        <v>145679</v>
+      </c>
+      <c r="AB24" s="26">
+        <v>145679</v>
+      </c>
+      <c r="AC24" s="36">
+        <v>8</v>
+      </c>
+      <c r="AD24" s="25">
+        <v>145679</v>
+      </c>
+      <c r="AE24" s="39">
+        <v>3</v>
+      </c>
+      <c r="AF24" s="24">
+        <v>145679</v>
+      </c>
+      <c r="AG24" s="25">
+        <v>2</v>
+      </c>
+      <c r="AH24" s="26">
+        <v>145679</v>
+      </c>
+      <c r="AK24" s="24">
+        <v>14569</v>
+      </c>
+      <c r="AL24" s="25">
+        <v>1457</v>
+      </c>
+      <c r="AM24" s="26">
+        <v>156</v>
+      </c>
+      <c r="AN24" s="36">
+        <v>8</v>
+      </c>
+      <c r="AO24" s="25">
+        <v>569</v>
+      </c>
+      <c r="AP24" s="39">
+        <v>3</v>
+      </c>
+      <c r="AQ24" s="24">
+        <v>1467</v>
+      </c>
+      <c r="AR24" s="25">
+        <v>2</v>
+      </c>
+      <c r="AS24" s="26">
+        <v>14579</v>
+      </c>
+      <c r="AU24" s="24">
+        <v>459</v>
+      </c>
+      <c r="AV24" s="25">
+        <v>1457</v>
+      </c>
+      <c r="AW24" s="26">
+        <v>15</v>
+      </c>
+      <c r="AX24" s="36">
+        <v>8</v>
+      </c>
+      <c r="AY24" s="9">
+        <v>6</v>
+      </c>
+      <c r="AZ24" s="39">
+        <v>3</v>
+      </c>
+      <c r="BA24" s="24">
+        <v>147</v>
+      </c>
+      <c r="BB24" s="25">
+        <v>2</v>
+      </c>
+      <c r="BC24" s="26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="29">
+        <v>6</v>
+      </c>
+      <c r="N25">
+        <v>7</v>
+      </c>
+      <c r="O25" s="27">
+        <v>123456789</v>
+      </c>
+      <c r="P25" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="Q25" s="29">
+        <v>123456789</v>
+      </c>
+      <c r="R25" s="37">
+        <v>123456789</v>
+      </c>
+      <c r="S25" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="T25" s="40">
+        <v>123456789</v>
+      </c>
+      <c r="U25" s="27">
+        <v>123456789</v>
+      </c>
+      <c r="V25" s="28">
+        <v>123456789</v>
+      </c>
+      <c r="W25" s="29">
+        <v>6</v>
+      </c>
+      <c r="Y25">
+        <v>7</v>
+      </c>
+      <c r="Z25" s="27">
+        <v>12345789</v>
+      </c>
+      <c r="AA25" s="28">
+        <v>12345789</v>
+      </c>
+      <c r="AB25" s="29">
+        <v>12345789</v>
+      </c>
+      <c r="AC25" s="37">
+        <v>12345789</v>
+      </c>
+      <c r="AD25" s="28">
+        <v>12345789</v>
+      </c>
+      <c r="AE25" s="40">
+        <v>12345789</v>
+      </c>
+      <c r="AF25" s="27">
+        <v>12345789</v>
+      </c>
+      <c r="AG25" s="28">
+        <v>12345789</v>
+      </c>
+      <c r="AH25" s="29">
+        <v>6</v>
+      </c>
+      <c r="AK25" s="27">
+        <v>1234589</v>
+      </c>
+      <c r="AL25" s="28">
+        <v>134578</v>
+      </c>
+      <c r="AM25" s="29">
+        <v>1235</v>
+      </c>
+      <c r="AN25" s="37">
+        <v>459</v>
+      </c>
+      <c r="AO25" s="28">
+        <v>23589</v>
+      </c>
+      <c r="AP25" s="40">
+        <v>1247</v>
+      </c>
+      <c r="AQ25" s="27">
+        <v>1478</v>
+      </c>
+      <c r="AR25" s="28">
+        <v>13578</v>
+      </c>
+      <c r="AS25" s="29">
+        <v>6</v>
+      </c>
+      <c r="AU25" s="27">
+        <v>358</v>
+      </c>
+      <c r="AV25" s="28">
+        <v>3578</v>
+      </c>
+      <c r="AW25" s="29">
+        <v>235</v>
+      </c>
+      <c r="AX25" s="49">
+        <v>4</v>
+      </c>
+      <c r="AY25" s="11">
+        <v>9</v>
+      </c>
+      <c r="AZ25" s="53">
+        <v>1</v>
+      </c>
+      <c r="BA25" s="27">
+        <v>78</v>
+      </c>
+      <c r="BB25" s="28">
+        <v>13578</v>
+      </c>
+      <c r="BC25" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="30">
+        <v>2</v>
+      </c>
+      <c r="G26" s="31">
+        <v>7</v>
+      </c>
+      <c r="H26" s="32">
+        <v>5</v>
+      </c>
+      <c r="I26" s="30">
+        <v>9</v>
+      </c>
+      <c r="J26" s="31"/>
+      <c r="K26" s="32"/>
+      <c r="N26">
+        <v>8</v>
+      </c>
+      <c r="O26" s="30">
+        <v>123456789</v>
+      </c>
+      <c r="P26" s="31">
+        <v>123456789</v>
+      </c>
+      <c r="Q26" s="32">
+        <v>123456789</v>
+      </c>
+      <c r="R26" s="38">
+        <v>2</v>
+      </c>
+      <c r="S26" s="31">
+        <v>7</v>
+      </c>
+      <c r="T26" s="41">
+        <v>5</v>
+      </c>
+      <c r="U26" s="30">
+        <v>9</v>
+      </c>
+      <c r="V26" s="31">
+        <v>123456789</v>
+      </c>
+      <c r="W26" s="32">
+        <v>123456789</v>
+      </c>
+      <c r="Y26">
+        <v>8</v>
+      </c>
+      <c r="Z26" s="30">
+        <v>13468</v>
+      </c>
+      <c r="AA26" s="31">
+        <v>13468</v>
+      </c>
+      <c r="AB26" s="32">
+        <v>13468</v>
+      </c>
+      <c r="AC26" s="38">
+        <v>2</v>
+      </c>
+      <c r="AD26" s="31">
+        <v>7</v>
+      </c>
+      <c r="AE26" s="41">
+        <v>5</v>
+      </c>
+      <c r="AF26" s="30">
+        <v>9</v>
+      </c>
+      <c r="AG26" s="31">
+        <v>13468</v>
+      </c>
+      <c r="AH26" s="32">
+        <v>13468</v>
+      </c>
+      <c r="AK26" s="30">
+        <v>13468</v>
+      </c>
+      <c r="AL26" s="31">
+        <v>1348</v>
+      </c>
+      <c r="AM26" s="32">
+        <v>136</v>
+      </c>
+      <c r="AN26" s="38">
+        <v>2</v>
+      </c>
+      <c r="AO26" s="31">
+        <v>7</v>
+      </c>
+      <c r="AP26" s="41">
+        <v>5</v>
+      </c>
+      <c r="AQ26" s="30">
+        <v>9</v>
+      </c>
+      <c r="AR26" s="31">
+        <v>1368</v>
+      </c>
+      <c r="AS26" s="32">
+        <v>1348</v>
+      </c>
+      <c r="AU26" s="30">
+        <v>3468</v>
+      </c>
+      <c r="AV26" s="31">
+        <v>1348</v>
+      </c>
+      <c r="AW26" s="32">
+        <v>136</v>
+      </c>
+      <c r="AX26" s="38">
+        <v>2</v>
+      </c>
+      <c r="AY26" s="31">
+        <v>7</v>
+      </c>
+      <c r="AZ26" s="41">
+        <v>5</v>
+      </c>
+      <c r="BA26" s="30">
+        <v>9</v>
+      </c>
+      <c r="BB26" s="31">
+        <v>138</v>
+      </c>
+      <c r="BC26" s="32">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>